<commit_message>
committing because i was too lazy too over the past couple of weeks
</commit_message>
<xml_diff>
--- a/app/data/db/master/Automation Data.xlsx
+++ b/app/data/db/master/Automation Data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\_Development\AssetManagementPortal\app\data\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nburmeister\Documents\_Development\AssetManagementPortal\app\data\db\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C50C8F9-8F69-48F1-9305-2C2240882F23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEACEF4B-48F4-42E5-BDB8-4CC0E9B5837B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="16440" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="16440" activeTab="1" xr2:uid="{65CCAB74-0CA2-4D5F-9FC7-1AACCFC26E43}"/>
   </bookViews>
   <sheets>
     <sheet name="PropertyData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
@@ -30,6 +30,7 @@
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
     <definedName name="______wrn1" hidden="1">{"schedule1",#N/A,FALSE,"Sheet1";"schedule2",#N/A,FALSE,"Sheet1";"schedule3",#N/A,FALSE,"Sheet1";"schedule4",#N/A,FALSE,"Sheet1";"schedule5",#N/A,FALSE,"Sheet1";"schedule6",#N/A,FALSE,"Sheet1"}</definedName>
@@ -42,6 +43,7 @@
     <definedName name="_e4" hidden="1">{"new",#N/A,FALSE,"D";"PROFORMA",#N/A,FALSE,"A";"partial 1",#N/A,FALSE,"B";"partial 2",#N/A,FALSE,"B";"partial 3",#N/A,FALSE,"B";"SMALL CF 1",#N/A,FALSE,"C"}</definedName>
     <definedName name="_Fill" hidden="1">[1]Avian!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PropertyData!$A$1:$AW$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Key2" hidden="1">#REF!</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
@@ -3523,7 +3525,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="335">
   <si>
     <t>Status</t>
   </si>
@@ -4472,6 +4474,63 @@
   <si>
     <t>Buildings</t>
   </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>18140</t>
+  </si>
+  <si>
+    <t>17140</t>
+  </si>
+  <si>
+    <t>33460</t>
+  </si>
+  <si>
+    <t>33340</t>
+  </si>
+  <si>
+    <t>36420</t>
+  </si>
+  <si>
+    <t>46140</t>
+  </si>
+  <si>
+    <t>19780</t>
+  </si>
+  <si>
+    <t>26420</t>
+  </si>
+  <si>
+    <t>37980</t>
+  </si>
+  <si>
+    <t>45300</t>
+  </si>
+  <si>
+    <t>38060</t>
+  </si>
+  <si>
+    <t>19100</t>
+  </si>
+  <si>
+    <t>10740</t>
+  </si>
+  <si>
+    <t>12060</t>
+  </si>
+  <si>
+    <t>28140</t>
+  </si>
+  <si>
+    <t>38300</t>
+  </si>
+  <si>
+    <t>23540</t>
+  </si>
+  <si>
+    <t>16980</t>
+  </si>
 </sst>
 </file>
 
@@ -59931,11 +59990,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7710D90B-EE59-4300-997E-0C7673234710}">
   <dimension ref="A1:AW104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2:I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68886,12 +68945,184 @@
       <c r="AA104" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AW74" xr:uid="{46105795-6248-483D-A056-3911B7690D43}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AW74">
-      <sortCondition ref="C1:C74"/>
+  <autoFilter ref="A1:AW74" xr:uid="{46105795-6248-483D-A056-3911B7690D43}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7798B693-97FF-4EEB-BB92-103FD8C867F5}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{711F4C36-1ADB-4828-9BEC-45F5A2C0087D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>